<commit_message>
me cago en la puta
</commit_message>
<xml_diff>
--- a/modelos deterministicos/modelo determenistico 2018-S1/programacion dinamica.xlsx
+++ b/modelos deterministicos/modelo determenistico 2018-S1/programacion dinamica.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\repap\Documents\Repositorios GIT\Jp_asig_2018-S2\modelos deterministicos\modelo determenistico 2018-S1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F466C-4A05-4269-A3C7-23AC52FFCD1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10,2,3" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -447,7 +454,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -745,7 +752,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -779,7 +786,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1073,10 +1086,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1449,10 +1462,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E28" workbookViewId="0">
       <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>

</xml_diff>